<commit_message>
Iteration 2 progress report
</commit_message>
<xml_diff>
--- a/doc/CS673_ProgressReport_team1.xlsx
+++ b/doc/CS673_ProgressReport_team1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="229">
   <si>
     <t xml:space="preserve">This report has 1 group iteration progress summary sheet to be filled at the end of each iteration by the team leader, 
 1 project ontribution sheet to be filled by everyone at the end of the semester, and 1 weekly report sheet per student. </t>
@@ -118,6 +118,51 @@
   </si>
   <si>
     <t xml:space="preserve">- For next iteration, we will set up the story and distribute it to each memebers </t>
+  </si>
+  <si>
+    <t>09/15-09/26</t>
+  </si>
+  <si>
+    <t>- Begin setting up the database
+- Begin creating pipeline
+- Begin creating authentication
+- Completed SDD
+- Completed STD</t>
+  </si>
+  <si>
+    <t>Deciding how to proceed with Authentication</t>
+  </si>
+  <si>
+    <t>- Team was sub-broken into front end team and back end team, each team then decided on certain approaches that team members planned to familiarize themselves with</t>
+  </si>
+  <si>
+    <t>- Have regular meetings to check in on code progress for all team members
+- Have multiple team members check to ensure they can access the different tools being used to set the project up</t>
+  </si>
+  <si>
+    <t>09/27-10/10</t>
+  </si>
+  <si>
+    <t>- Created endpoints for front end to access database
+- Created functionality code in backend that enables our core features
+- Decided on authentication and began working that into the program
+- Decided on front end framework (MUI)
+- Began creating components for UI
+- Created pipeline
+- Created container
+- Decided on using Hiroku as our hosting tool
+- Connected Hiroku to backend
+- Created and tested dashboard, set up, navigation, add expense, and add income components</t>
+  </si>
+  <si>
+    <t>- With team members beginning to access code from other areas of the program, the team had to communicate across front end and back end teams to ensure that all of the needed endpoints were accessible. 
+- Additionally, due to the combination of front end and back end progress, the team had to work together to create new endpoints for certain requirements and had to communicate more with different members to ensure the front end could communicate properly with the backend. 
+- Since we need to have the application hosted for the final iteration, the team needed to find a hosting tool and ensure that it would integrate with our setup without having to invest too much time to ensure other application requirements were met</t>
+  </si>
+  <si>
+    <t>- Integrate the Hiroku hosting with the front end for the final iteration
+- Continue testing components to ensure database is updated for particular users
+- Finalize the notification feature that will monitor expense categories and alert users when a category has exceeded a determined limit</t>
   </si>
   <si>
     <t>This sheet need to be filled by the end of the semester. You should clearly describe your contribution to 
@@ -296,6 +341,67 @@
     <t>Na</t>
   </si>
   <si>
+    <t>9/19 - 09/25</t>
+  </si>
+  <si>
+    <t>0 - learn Database; Learn cucumber testing
+1 - Work with the team to plan high-level architectural design of project
+2 - Created design patterns to be implemented
+5 - communication with team and meetings; up the timeline for our requirements
+7 - Updated documentation, created and presented Iteration 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design pattern </t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Start implementation of budget notification system</t>
+  </si>
+  <si>
+    <t>9/25- 10/02</t>
+  </si>
+  <si>
+    <t>0 - learn Database; Learn cucumber testing
+1 - Work with the team to plan high-level architectural design of project
+3- started working on budget notification system
+5 - communication with team and meetings; up the timeline for our requirements
+7 - Updated documentation</t>
+  </si>
+  <si>
+    <t>Budget notification system and testing</t>
+  </si>
+  <si>
+    <t>1. errors not letting compile</t>
+  </si>
+  <si>
+    <t>reviewed code with team and found imports missing</t>
+  </si>
+  <si>
+    <t>finsish budgeting notifications system and start on testing</t>
+  </si>
+  <si>
+    <t>10/03- 10/10</t>
+  </si>
+  <si>
+    <t>0 - learn Database; Learn cucumber testing
+1 - Work with the team to plan high-level architectural design of project
+3- working on budget notification system
+4- creating tests for budget notifcation
+5 - communication with team and meetings; up the timeline for our requirements
+7 - Updated documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on testing will merge with dev branch after </t>
+  </si>
+  <si>
+    <t>implementation completed, working on creating tests</t>
+  </si>
+  <si>
+    <t>finish testing. see if team wants to add budgeting option by category</t>
+  </si>
+  <si>
     <t>Sean Rawson</t>
   </si>
   <si>
@@ -388,6 +494,41 @@
     <t>1. Continue implementation of endpoints
 2. Move forward with authentication system development
 3. Discuss communication between front and back-end components with team</t>
+  </si>
+  <si>
+    <t>09/26 - 10/02</t>
+  </si>
+  <si>
+    <t>2 - Design user overview endpoint to support UI dashboard
+3 - Refine API endpoints and add additional ones as needed to support front end functionality
+4 - Write unit tests for main back end classes
+5 - Group meetings/discord communication</t>
+  </si>
+  <si>
+    <t>No issues</t>
+  </si>
+  <si>
+    <t>1. Help integrated authentication code with existing back end
+2. Continue writing unit tests</t>
+  </si>
+  <si>
+    <t>10/3 - 10/9</t>
+  </si>
+  <si>
+    <t>0 - Learn about JPA interaction with composite primary key tables
+2 - Design classes and database table for expense category budgets in preparation for iteration 3
+3 - Implement date range searches for expense, income, and user overview endpoints
+4 - Continue filling out unit tests for the back end
+5 - Assist in testing efforts for planned expense notification functionality, communicate with team about database updates</t>
+  </si>
+  <si>
+    <t>Updated SPPP risk management spreadsheet
+Personal progress report</t>
+  </si>
+  <si>
+    <t>1. Help integrate front end with back end
+2. Perform testing to ensure that authentication functionality integrates well with back end
+3. Add expense category budgeting options to back end</t>
   </si>
   <si>
     <r>
@@ -486,6 +627,55 @@
 5. Write up documentation how to run the containers </t>
   </si>
   <si>
+    <t>09/26-10/2</t>
+  </si>
+  <si>
+    <t>0 - learn about render as Yuting suggested
+6 - Merging branches to keep code 
+7 - Investigate why upload to google drive stoopped working
+7. Investigate using Render as a new platform to deploy</t>
+  </si>
+  <si>
+    <t>1. Investigate uploading zip file to google drive stopped working - abandon using this method
+2. Trying to switch to use Render as Yuting suggested
+3. Determined Render is not a good platform for our project
+4. Switch to Heroku</t>
+  </si>
+  <si>
+    <t>1. Learn Heroku and how the platform works</t>
+  </si>
+  <si>
+    <t>10/3-10/9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 - learn Heroku platform
+2 - design how to deploy to Heroku
+3 - set up the backend deployment to Heroku
+3 - set up the application container
+3 - Implement secret for deployment 
+4 - testing the deployment
+5 - work with Jisoo/mali/Sean on the front end deployment and the backend
+6 - Configuring MariaDB on Heroku
+7 - Investigate build pack issues
+7 - investigate different DB addon. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Switched to deploy to Heroku as google drive failed working
+2. Set up new action to accomodate the change
+3. </t>
+  </si>
+  <si>
+    <t>1. Need to resolve the port number for backend (Heroku assigns random #) - resolved
+2. Heroku offers many ways to deploy and have to pick out the right method 
+3. git structure need to accomodate (as build pack does not work with sub folders) - resolved
+4. Mainly on debugging the deployment as Heroku throws deployment errors for the back end - resolved</t>
+  </si>
+  <si>
+    <t>1. Deploy Front End
+2. Work with Front end team to hook up bankend endpoint in production environment
+3. Work with database for changes Sean requested</t>
+  </si>
+  <si>
     <t>Mali Rivera</t>
   </si>
   <si>
@@ -577,6 +767,51 @@
 3 - implement front-end functionality  </t>
   </si>
   <si>
+    <t>Individual Task Breakdown
+0 - Learn Material UI, Chart.js, mockMVC, and mockito, learn how to integrate spring boot and react
+3- Work on Dashboard.js, NavBar.js, ExpenseChart.js and ExpenseTable.js
+4 - Write Integration tests   
+5 - help communicate how to run project locally, and access backend on front-end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. write Lab 3 code  
+2. write integration tests  3. enabled CORS configuration so that front-end can access code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. not familiar with integrating back end and front end and working with local databases 
+2. not familiar with spring boot so have to research controller vs. service vs. mapper to be able to write tests </t>
+  </si>
+  <si>
+    <t>need to research more about spring boot and react integration, and also integration testing with spring mock MVC</t>
+  </si>
+  <si>
+    <t>0 - continue to work on back end and front end integration 
+1 - work on front-end implementation of user stories 
+3 - write tests</t>
+  </si>
+  <si>
+    <t>Individual Task Breakdown
+0 - learn Material UI, Chart.js, mockMVC, and mockito
+3- Integrate back and front end, add logic to create a map of user expenses by expenseCategory, pull data in front-end, check posting data updates charts in real time, add integration tests, create demo for front-end slides 
+4 - write Integration tests, write STD sections, create Testing Metrics Report, create Testing Slides for presentation 
+5 - help communicate how to run project locally, and access backend on front-end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. code (Dashboard.js, ExpenseChart.js, ExpenseTable.js, NavBar.js, Integration tests) 
+2. create Testing Metrics Report, Testing slides, STD update, and script testing slides, record front-end demo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">we're having issues with login functionality which affects the implementation of the rest of our program </t>
+  </si>
+  <si>
+    <t>need to figure out a login plan with the team, add date filtering capability to dashboard, edit the UI design, make sure we have all the functinoality that we wanted and continue to write tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 - continue to work on back end and front end integration 
+1 - finish up front-end implementation 
+3 - continue to test, study for final </t>
+  </si>
+  <si>
     <t>Sherif Zeyada</t>
   </si>
   <si>
@@ -598,6 +833,32 @@
   </si>
   <si>
     <t>1. Wrote out high level requirements proposal for SPPP</t>
+  </si>
+  <si>
+    <t>0 - Research Google Oauth2
+2 - Plan initial Google Oauth2
+3 - Create Google confidentail
+5 - Discuss high-level architecture with team</t>
+  </si>
+  <si>
+    <t>0 - Continue learning about google authentication and spring security
+2 - Work with team to plan high level architectural design of project
+4 - Write first unit tests
+5 - Meet with Saan to discuss authentication, coordinate with team regarding iteration 1 presentation</t>
+  </si>
+  <si>
+    <t>SDD Design and database</t>
+  </si>
+  <si>
+    <t>0 - Learn about React
+2 - Design the integration between the Frontend and backend google Oauth
+4 - Continue filling out unit tests for the back end
+5 - Assist in testing communicate with team about database updates</t>
+  </si>
+  <si>
+    <t>1. Help integrate front end with back end
+2. Perform testing to ensure that authentication functionality integrates well with back end
+3</t>
   </si>
   <si>
     <r>
@@ -691,6 +952,65 @@
 6 - Ensure that we have a universal staging environment that we can all reference and see how the project is progressing </t>
   </si>
   <si>
+    <t>09/26 - 10/2</t>
+  </si>
+  <si>
+    <t>0 - Learn about postman, docker, material ui, accessing endpoints, creating local environment for development
+1 - Bi-weekly code checkins to ensure progress is being made and team members feel comfortable about their workload
+2 - Using components from MUI, designed the layout for the add-expense and add-income pages
+5 - Created outlines for each of our meetings, checked in with all team members at each meeting to see how progress is coming along, ensured that team members feel comfortable with their workload</t>
+  </si>
+  <si>
+    <t>1. Learned how to work with MUI and began creating the AddIncome and AddExpense pages</t>
+  </si>
+  <si>
+    <t>1. Overall very unsure about a lot of the programs that we're using so a bulk of time this week was spent learning how to use those and work with them efficiently</t>
+  </si>
+  <si>
+    <t>1. Continue learning about these programs and work with a couple of small examples to familiarize myself before applying that information directly to our working project</t>
+  </si>
+  <si>
+    <t>0 - continue learning about pipeline, docker, and mariaDB
+3 - create the AddIncome and AddExpense components
+5 - continue leading meetings and checking in with team members
+6 - plan to successfully set up a local environment for testing</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">0 - Continued learning Docker and MUI
+1 - Wrote </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Readme.md</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> file to outline how to use the application + Reviewed SPPP and provided comments on all features that have had progress made for this iteration
+2 - Continued designing the layout for the AddExpense and AddIncome pages
+3 - Commited AddExpense and AddIncome components to working branch
+5 - Created outlines for each meeting, checked in with team members, led meetings
+6 - Was able to successfully create a local environment</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Created the AddIncome and AddExpense components
+2. Wrote readme file and updated SPPP document to cover progress
+3 - Finished creating the AddIncome and AddExpense
+4 - Ensured that the two components were working locally
+5 - Continued leading meetings and ensuring that we had an outline to reference for meetups
+6 - Set up local environment and was able to run docker</t>
+  </si>
+  <si>
+    <t>0 - continue learning about the pipeline and Hiroku for our final iteration
+3 - Finalize the AddIncome and AddExpense to ensure it is working properly
+5 - continue leading meetings</t>
+  </si>
+  <si>
     <t>Jisoo Lee</t>
   </si>
   <si>
@@ -782,12 +1102,65 @@
 2 - Team work with front-end design
 6 - Set up VScode, React libraries</t>
   </si>
+  <si>
+    <t>0 - Continue learning Google Oauth in Javascript
+1 - Updated accepatance test for requirements and set up the timeline for our requirements
+3 - Work on the front end, user set up page 
+4 - Work on Lab3 test on Javascript code
+5 - Meet with Brian and Mali with front-end. Regular meeting with whole team to ensure design for full stack application 
+5 - Set up VScode, intall Node.js and React. Distributed pages for the frontend team.</t>
+  </si>
+  <si>
+    <t>1. Testing javascript for Lab3
+2. Install Node.js React app and created pages. 
+3. Updated Jira status</t>
+  </si>
+  <si>
+    <t>1. Installing React app and integrating with backend required a lot of communication
+2. Need to work with backend team with the Google Oauth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Continue to work on Google Oauth process in frontend </t>
+  </si>
+  <si>
+    <t>1- Update status in Jira 
+1 - Update SPPP and STD accpetance test 
+2 - Team work with front-end design 
+3 - Write code for SetUp page and Login page
+4 - communicate with backend for checking endpoints for REST APIs and work with conficurations set ups for deploying</t>
+  </si>
+  <si>
+    <t>10/03 - 10/09</t>
+  </si>
+  <si>
+    <t>0 - Continue learning Google Oauth in Javascript
+1 - Updated Jira time line 
+3 - Work on the front end, updating user set up page and Google Oauth
+4 - Testing whether it is integrated with backend.
+5 - Meet with Brian and Mali with front-end. Regular meeting with whole team to ensure design for full stack application, presentation recording for iteration2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Write code for Sign-in folder (SetUp.js, Auth.js, Login.js, OauthRedirect.js, PostToken.js)
+2. Check endpoints for REST APIs with backend team and updated the codes
+3. Presentation for interation2 mock up video for frontend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Integration with backend required loads of communications for updating bugs
+2. Need to work on Google Oauth with back end team </t>
+  </si>
+  <si>
+    <t>1- Update status in Jira and check the progress
+1 - Update SPPP and STD
+2 - Team work with front-end design 
+3 - Write code for user name set ups when Google Oauth is ready
+4 - communicate with backend for checking endpoints for REST APIs and work with conficurations set ups for deploying</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -835,12 +1208,20 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <b/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -851,6 +1232,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -874,7 +1261,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -950,8 +1337,14 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1211,7 +1604,7 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="12.63"/>
     <col customWidth="1" min="3" max="3" width="33.5"/>
-    <col customWidth="1" min="4" max="4" width="22.13"/>
+    <col customWidth="1" min="4" max="4" width="43.25"/>
     <col customWidth="1" min="5" max="5" width="25.75"/>
     <col customWidth="1" min="6" max="6" width="22.25"/>
     <col customWidth="1" min="7" max="7" width="9.88"/>
@@ -1439,19 +1832,35 @@
       <c r="A5" s="7">
         <v>1.0</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="9">
+        <v>5.0</v>
+      </c>
       <c r="L5" s="10">
         <f t="shared" si="1"/>
-        <v>43.5</v>
+        <v>52</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="2"/>
-        <v>43.5</v>
+        <v>52</v>
       </c>
       <c r="O5" s="10">
         <f>SUM('Chaitanya Saraogi'!G5+'Sean Rawson'!G5+'Clyde Yeung'!G5+'Mali Rivera'!G5+'Sherif Zeyada'!G5+'Brian Fenstermacher'!G5+'Jisoo Lee'!G6)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="P5" s="10">
         <f>SUM('Chaitanya Saraogi'!H5+'Sean Rawson'!H5+'Clyde Yeung'!H5+'Mali Rivera'!H5+'Sherif Zeyada'!H5+'Brian Fenstermacher'!H5+'Jisoo Lee'!H6)</f>
@@ -1459,11 +1868,11 @@
       </c>
       <c r="Q5" s="10">
         <f>SUM('Chaitanya Saraogi'!I5+'Sean Rawson'!I5+'Clyde Yeung'!I5+'Mali Rivera'!I5+'Sherif Zeyada'!I5+'Brian Fenstermacher'!I5+'Jisoo Lee'!I6)</f>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="R5" s="10">
         <f>SUM('Chaitanya Saraogi'!J5+'Sean Rawson'!J5+'Clyde Yeung'!J5+'Mali Rivera'!J5+'Sherif Zeyada'!J5+'Brian Fenstermacher'!J5+'Jisoo Lee'!J6)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S5" s="10">
         <f>SUM('Chaitanya Saraogi'!K5+'Sean Rawson'!K5+'Clyde Yeung'!K5+'Mali Rivera'!K5+'Sherif Zeyada'!K5+'Brian Fenstermacher'!K5+'Jisoo Lee'!K6)</f>
@@ -1471,7 +1880,7 @@
       </c>
       <c r="T5" s="10">
         <f>SUM('Chaitanya Saraogi'!L5+'Sean Rawson'!L5+'Clyde Yeung'!L5+'Mali Rivera'!L5+'Sherif Zeyada'!L5+'Brian Fenstermacher'!L5+'Jisoo Lee'!L6)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U5" s="10">
         <f>SUM('Chaitanya Saraogi'!M5+'Sean Rawson'!M5+'Clyde Yeung'!M5+'Mali Rivera'!M5+'Sherif Zeyada'!M5+'Brian Fenstermacher'!M5+'Jisoo Lee'!M6)</f>
@@ -1486,39 +1895,59 @@
       <c r="A6" s="7">
         <v>2.0</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>3.0</v>
+      </c>
       <c r="L6" s="10">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>76.5</v>
       </c>
       <c r="M6" s="10">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>76.5</v>
       </c>
       <c r="O6" s="10">
         <f>SUM('Chaitanya Saraogi'!G6+'Sean Rawson'!G6+'Clyde Yeung'!G6+'Mali Rivera'!G6+'Sherif Zeyada'!G6+'Brian Fenstermacher'!G6+'Jisoo Lee'!G7)</f>
-        <v>10.5</v>
+        <v>19</v>
       </c>
       <c r="P6" s="10">
         <f>SUM('Chaitanya Saraogi'!H6+'Sean Rawson'!H6+'Clyde Yeung'!H6+'Mali Rivera'!H6+'Sherif Zeyada'!H6+'Brian Fenstermacher'!H6+'Jisoo Lee'!H7)</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q6" s="10">
         <f>SUM('Chaitanya Saraogi'!I6+'Sean Rawson'!I6+'Clyde Yeung'!I6+'Mali Rivera'!I6+'Sherif Zeyada'!I6+'Brian Fenstermacher'!I6+'Jisoo Lee'!I7)</f>
-        <v>2.5</v>
+        <v>6.5</v>
       </c>
       <c r="R6" s="10">
         <f>SUM('Chaitanya Saraogi'!J6+'Sean Rawson'!J6+'Clyde Yeung'!J6+'Mali Rivera'!J6+'Sherif Zeyada'!J6+'Brian Fenstermacher'!J6+'Jisoo Lee'!J7)</f>
-        <v>20.5</v>
+        <v>26.5</v>
       </c>
       <c r="S6" s="10">
         <f>SUM('Chaitanya Saraogi'!K6+'Sean Rawson'!K6+'Clyde Yeung'!K6+'Mali Rivera'!K6+'Sherif Zeyada'!K6+'Brian Fenstermacher'!K6+'Jisoo Lee'!K7)</f>
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="T6" s="10">
         <f>SUM('Chaitanya Saraogi'!L6+'Sean Rawson'!L6+'Clyde Yeung'!L6+'Mali Rivera'!L6+'Sherif Zeyada'!L6+'Brian Fenstermacher'!L6+'Jisoo Lee'!L7)</f>
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="U6" s="10">
         <f>SUM('Chaitanya Saraogi'!M6+'Sean Rawson'!M6+'Clyde Yeung'!M6+'Mali Rivera'!M6+'Sherif Zeyada'!M6+'Brian Fenstermacher'!M6+'Jisoo Lee'!M7)</f>
@@ -1526,7 +1955,7 @@
       </c>
       <c r="V6" s="10">
         <f>SUM('Chaitanya Saraogi'!N6+'Sean Rawson'!N6+'Clyde Yeung'!N6+'Mali Rivera'!N6+'Sherif Zeyada'!N6+'Brian Fenstermacher'!N6+'Jisoo Lee'!N7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -1537,47 +1966,47 @@
       <c r="C7" s="7"/>
       <c r="L7" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="M7" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="O7" s="10">
         <f>SUM('Chaitanya Saraogi'!G7+'Sean Rawson'!G7+'Clyde Yeung'!G7+'Mali Rivera'!G7+'Sherif Zeyada'!G7+'Brian Fenstermacher'!G7+'Jisoo Lee'!G8)</f>
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="P7" s="10">
         <f>SUM('Chaitanya Saraogi'!H7+'Sean Rawson'!H7+'Clyde Yeung'!H7+'Mali Rivera'!H7+'Sherif Zeyada'!H7+'Brian Fenstermacher'!H7+'Jisoo Lee'!H8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="10">
         <f>SUM('Chaitanya Saraogi'!I7+'Sean Rawson'!I7+'Clyde Yeung'!I7+'Mali Rivera'!I7+'Sherif Zeyada'!I7+'Brian Fenstermacher'!I7+'Jisoo Lee'!I8)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R7" s="10">
         <f>SUM('Chaitanya Saraogi'!J7+'Sean Rawson'!J7+'Clyde Yeung'!J7+'Mali Rivera'!J7+'Sherif Zeyada'!J7+'Brian Fenstermacher'!J7+'Jisoo Lee'!J8)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S7" s="10">
         <f>SUM('Chaitanya Saraogi'!K7+'Sean Rawson'!K7+'Clyde Yeung'!K7+'Mali Rivera'!K7+'Sherif Zeyada'!K7+'Brian Fenstermacher'!K7+'Jisoo Lee'!K8)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T7" s="10">
         <f>SUM('Chaitanya Saraogi'!L7+'Sean Rawson'!L7+'Clyde Yeung'!L7+'Mali Rivera'!L7+'Sherif Zeyada'!L7+'Brian Fenstermacher'!L7+'Jisoo Lee'!L8)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U7" s="10">
         <f>SUM('Chaitanya Saraogi'!M7+'Sean Rawson'!M7+'Clyde Yeung'!M7+'Mali Rivera'!M7+'Sherif Zeyada'!M7+'Brian Fenstermacher'!M7+'Jisoo Lee'!M8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="10">
         <f>SUM('Chaitanya Saraogi'!N7+'Sean Rawson'!N7+'Clyde Yeung'!N7+'Mali Rivera'!N7+'Sherif Zeyada'!N7+'Brian Fenstermacher'!N7+'Jisoo Lee'!N8)</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
     </row>
@@ -2618,8 +3047,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>136</v>
+      <c r="A1" s="28" t="s">
+        <v>202</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -2645,7 +3074,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -2666,22 +3095,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -2708,19 +3137,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -2735,7 +3164,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C4" s="21">
         <f>D4+E4</f>
@@ -2749,7 +3178,7 @@
         <v>2.0</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="G4" s="24">
         <v>1.0</v>
@@ -2776,16 +3205,16 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>141</v>
+        <v>207</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="S4" s="21">
         <v>6.0</v>
@@ -2803,7 +3232,7 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" s="9">
         <v>5.5</v>
@@ -2815,7 +3244,7 @@
         <v>1.5</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>143</v>
+        <v>209</v>
       </c>
       <c r="G5" s="8">
         <v>1.5</v>
@@ -2842,16 +3271,16 @@
         <v>0.0</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>146</v>
+        <v>212</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="S5" s="8">
         <v>6.0</v>
@@ -2865,7 +3294,7 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C6" s="9">
         <v>5.5</v>
@@ -2877,7 +3306,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="G6" s="8">
         <v>1.5</v>
@@ -2904,16 +3333,16 @@
         <v>0.0</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>149</v>
+        <v>215</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>150</v>
+        <v>216</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
       <c r="S6" s="8">
         <v>6.0</v>
@@ -2923,36 +3352,120 @@
       <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="9">
+        <v>10.5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>8.0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="R7" s="29" t="s">
+        <v>223</v>
+      </c>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="A8" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="9">
+        <v>13.5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>9.0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="R8" s="29" t="s">
+        <v>228</v>
+      </c>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
@@ -8612,11 +9125,12 @@
     <col customWidth="1" min="3" max="3" width="15.88"/>
     <col customWidth="1" min="4" max="5" width="12.63"/>
     <col customWidth="1" min="6" max="6" width="10.63"/>
+    <col customWidth="1" min="8" max="8" width="14.25"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.0" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -8646,37 +9160,37 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="14" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
@@ -9730,7 +10244,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -9756,7 +10270,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="19" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -9777,22 +10291,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -9819,19 +10333,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -9846,7 +10360,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C4" s="21">
         <f>D4+E4</f>
@@ -9860,7 +10374,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G4" s="21">
         <v>3.0</v>
@@ -9881,16 +10395,16 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S4" s="21">
         <v>6.0</v>
@@ -14612,7 +15126,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -14638,7 +15152,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -14659,22 +15173,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -14701,19 +15215,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -14728,10 +15242,10 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C4" s="21">
-        <f t="shared" ref="C4:C5" si="1">D4+E4</f>
+        <f t="shared" ref="C4:C8" si="1">D4+E4</f>
         <v>4</v>
       </c>
       <c r="D4" s="21">
@@ -14742,7 +15256,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G4" s="24">
         <v>2.0</v>
@@ -14759,16 +15273,16 @@
       </c>
       <c r="N4" s="21"/>
       <c r="O4" s="24" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="S4" s="21">
         <v>6.0</v>
@@ -14782,8 +15296,11 @@
       <c r="Z4" s="22"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9">
+        <v>2.0</v>
+      </c>
       <c r="B5" s="24" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" si="1"/>
@@ -14796,7 +15313,7 @@
         <v>1.0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G5" s="8">
         <v>2.0</v>
@@ -14811,70 +15328,196 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="S5" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="A6" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="21">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D6" s="9">
+        <v>9.0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2.0</v>
+      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="L6" s="8">
+        <v>1.0</v>
+      </c>
       <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+      <c r="N6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S6" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
       <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="21">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>8.0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="S7" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="B8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="21">
+        <f t="shared" si="1"/>
+        <v>11.5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>9.0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="S8" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -19498,7 +20141,7 @@
     <col customWidth="1" min="3" max="3" width="7.25"/>
     <col customWidth="1" min="4" max="4" width="8.38"/>
     <col customWidth="1" min="5" max="5" width="7.13"/>
-    <col customWidth="1" min="6" max="6" width="32.5"/>
+    <col customWidth="1" min="6" max="6" width="33.38"/>
     <col customWidth="1" min="7" max="7" width="5.63"/>
     <col customWidth="1" min="8" max="8" width="5.75"/>
     <col customWidth="1" min="9" max="9" width="5.88"/>
@@ -19516,7 +20159,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -19542,7 +20185,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -19563,22 +20206,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -19605,19 +20248,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -19632,13 +20275,15 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="21"/>
+        <v>70</v>
+      </c>
+      <c r="C4" s="24">
+        <v>4.0</v>
+      </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="24" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="G4" s="24">
         <v>2.0</v>
@@ -19665,16 +20310,16 @@
         <v>0.0</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="S4" s="24">
         <v>4.0</v>
@@ -19692,10 +20337,13 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8.5</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="G5" s="8">
         <v>4.0</v>
@@ -19722,16 +20370,16 @@
         <v>0.0</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="S5" s="8">
         <v>8.0</v>
@@ -19745,10 +20393,13 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>83</v>
+        <v>108</v>
+      </c>
+      <c r="C6" s="9">
+        <v>11.5</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="G6" s="8">
         <v>4.0</v>
@@ -19775,16 +20426,16 @@
         <v>0.0</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="S6" s="8">
         <v>10.0</v>
@@ -19794,37 +20445,113 @@
       <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="S7" s="8">
+        <v>8.0</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="A8" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="S8" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -24466,7 +25193,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -24492,7 +25219,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -24513,22 +25240,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -24555,19 +25282,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -24582,7 +25309,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C4" s="24">
         <v>8.0</v>
@@ -24594,7 +25321,7 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="G4" s="24">
         <v>4.0</v>
@@ -24617,16 +25344,16 @@
         <v>1.0</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
       <c r="S4" s="24">
         <v>12.0</v>
@@ -24644,7 +25371,7 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" s="9">
         <v>15.0</v>
@@ -24656,7 +25383,7 @@
         <v>2.0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="G5" s="8">
         <v>8.0</v>
@@ -24673,7 +25400,7 @@
         <v>3.0</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
@@ -24688,19 +25415,19 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C6" s="9">
         <v>25.0</v>
       </c>
       <c r="D6" s="9">
-        <v>25.0</v>
+        <v>23.0</v>
       </c>
       <c r="E6" s="9">
         <v>2.0</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="G6" s="8">
         <v>3.0</v>
@@ -24721,16 +25448,16 @@
         <v>3.0</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="S6" s="8">
         <v>25.0</v>
@@ -24740,42 +25467,115 @@
       <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20.0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>18.0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="8">
+        <v>7.0</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="L7" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>10.0</v>
+      </c>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="Q7" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="S7" s="8">
+        <v>30.0</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
+      <c r="A8" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>27.0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="8">
+        <v>8.0</v>
+      </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="I8" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="Q8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S8" s="8">
+        <v>25.0</v>
+      </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
+      <c r="F9" s="2"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -29412,7 +30212,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -29438,7 +30238,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -29459,22 +30259,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -29501,19 +30301,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -29528,7 +30328,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C4" s="24">
         <v>7.0</v>
@@ -29540,7 +30340,7 @@
         <v>2.0</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="G4" s="24">
         <v>2.0</v>
@@ -29561,16 +30361,16 @@
         <v>1.0</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="S4" s="21">
         <v>6.0</v>
@@ -29588,7 +30388,7 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" s="9">
         <v>7.5</v>
@@ -29600,7 +30400,7 @@
         <v>2.0</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="G5" s="8">
         <v>2.0</v>
@@ -29619,16 +30419,16 @@
         <v>2.0</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="S5" s="8">
         <v>6.0</v>
@@ -29637,12 +30437,12 @@
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
     </row>
-    <row r="6" ht="87.0" customHeight="1">
+    <row r="6" ht="101.25" customHeight="1">
       <c r="A6" s="9">
         <v>3.0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C6" s="9">
         <v>7.5</v>
@@ -29654,7 +30454,7 @@
         <v>2.0</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="G6" s="8">
         <v>2.0</v>
@@ -29673,16 +30473,16 @@
         <v>2.0</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="S6" s="8">
         <v>6.0</v>
@@ -29691,38 +30491,110 @@
       <c r="U6" s="7"/>
       <c r="V6" s="7"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
+    <row r="7" ht="101.25" customHeight="1">
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="G7" s="8">
+        <v>4.0</v>
+      </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>2.0</v>
+      </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="N7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="S7" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
+    <row r="8" ht="133.5" customHeight="1">
+      <c r="A8" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" s="8">
+        <v>4.0</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2.0</v>
+      </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="N8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="S8" s="8">
+        <v>13.0</v>
+      </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -34364,7 +35236,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -34390,7 +35262,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -34411,22 +35283,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -34453,19 +35325,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -34480,7 +35352,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C4" s="21">
         <f>D4+E4</f>
@@ -34494,7 +35366,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G4" s="21">
         <v>3.0</v>
@@ -34515,16 +35387,16 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="S4" s="21">
         <v>6.0</v>
@@ -34538,73 +35410,225 @@
       <c r="Z4" s="22"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="A5" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="S5" s="8">
+        <v>8.0</v>
+      </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+      <c r="A6" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="9">
+        <v>11.5</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="S6" s="8">
+        <v>10.0</v>
+      </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
       <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="S7" s="8">
+        <v>8.0</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="A8" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="S8" s="8">
+        <v>11.0</v>
+      </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -39224,11 +40248,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.0"/>
-    <col customWidth="1" min="2" max="2" width="10.13"/>
-    <col customWidth="1" min="3" max="3" width="7.25"/>
-    <col customWidth="1" min="4" max="4" width="8.38"/>
+    <col customWidth="1" min="2" max="2" width="12.5"/>
+    <col customWidth="1" min="3" max="3" width="24.38"/>
+    <col customWidth="1" min="4" max="4" width="18.25"/>
     <col customWidth="1" min="5" max="5" width="7.13"/>
-    <col customWidth="1" min="6" max="6" width="63.5"/>
+    <col customWidth="1" min="6" max="6" width="66.25"/>
     <col customWidth="1" min="7" max="7" width="6.13"/>
     <col customWidth="1" min="8" max="8" width="6.0"/>
     <col customWidth="1" min="9" max="9" width="5.88"/>
@@ -39236,7 +40260,7 @@
     <col customWidth="1" min="11" max="11" width="5.75"/>
     <col customWidth="1" min="12" max="13" width="6.0"/>
     <col customWidth="1" min="14" max="14" width="5.63"/>
-    <col customWidth="1" min="15" max="15" width="24.88"/>
+    <col customWidth="1" min="15" max="15" width="55.13"/>
     <col customWidth="1" min="16" max="16" width="19.63"/>
     <col customWidth="1" min="17" max="17" width="23.5"/>
     <col customWidth="1" min="18" max="18" width="56.38"/>
@@ -39246,7 +40270,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -39272,7 +40296,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -39293,22 +40317,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
@@ -39335,19 +40359,19 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -39362,7 +40386,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C4" s="21">
         <f>D4+E4</f>
@@ -39376,7 +40400,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G4" s="21">
         <v>3.0</v>
@@ -39397,16 +40421,16 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="S4" s="21">
         <v>6.0</v>
@@ -39424,7 +40448,7 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" s="9">
         <v>6.0</v>
@@ -39436,7 +40460,7 @@
         <v>2.0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="G5" s="8">
         <v>1.5</v>
@@ -39463,16 +40487,16 @@
         <v>0.0</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>128</v>
+        <v>185</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="S5" s="8">
         <v>5.0</v>
@@ -39486,7 +40510,7 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C6" s="9">
         <v>7.0</v>
@@ -39498,7 +40522,7 @@
         <v>2.0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="G6" s="8">
         <v>1.5</v>
@@ -39525,16 +40549,16 @@
         <v>0.0</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="S6" s="8">
         <v>6.0</v>
@@ -39544,37 +40568,109 @@
       <c r="V6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="A7" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="9">
+        <v>11.0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>8.0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="G7" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4.0</v>
+      </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8">
+        <v>1.0</v>
+      </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="O7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="S7" s="8">
+        <v>11.0</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="A8" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="9">
+        <v>14.5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>11.5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1.0</v>
+      </c>
       <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="O8" s="8" t="s">
+        <v>200</v>
+      </c>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="R8" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="S8" s="8">
+        <v>11.5</v>
+      </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -44179,6 +45275,9 @@
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="F8"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>